<commit_message>
Updating requirements.txt to include xlrd 1.2.0
</commit_message>
<xml_diff>
--- a/data/dfl_excel.xlsx
+++ b/data/dfl_excel.xlsx
@@ -388,13 +388,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4841577547543746</v>
+        <v>1.718974849135873</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1418688340412547</v>
+        <v>-0.05066157383224272</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2418840981520709</v>
+        <v>0.6452828968948781</v>
       </c>
     </row>
     <row r="3">
@@ -402,13 +402,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.259744537714209</v>
+        <v>0.363000991799871</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1198202402804975</v>
+        <v>0.4753304334074437</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.311022680284774</v>
+        <v>-0.4791181933660784</v>
       </c>
     </row>
     <row r="4">
@@ -416,13 +416,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.230095175707575</v>
+        <v>-0.8330479243490954</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9251788214463598</v>
+        <v>-1.024541131397955</v>
       </c>
       <c r="D4" t="n">
-        <v>1.174048052187721</v>
+        <v>-0.850531605951097</v>
       </c>
     </row>
     <row r="5">
@@ -430,13 +430,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.615007805343587</v>
+        <v>-1.569642914610615</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.07106345591559086</v>
+        <v>-0.0931295833021941</v>
       </c>
       <c r="D5" t="n">
-        <v>1.186953437751392</v>
+        <v>1.497903240195856</v>
       </c>
     </row>
     <row r="6">
@@ -444,13 +444,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.403878837274891</v>
+        <v>-0.8567210179775577</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.9268078081870629</v>
+        <v>1.614784838779701</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.9433935711317795</v>
+        <v>0.6441090578393747</v>
       </c>
     </row>
     <row r="7">
@@ -458,13 +458,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.2639846959320681</v>
+        <v>1.608110189805712</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5274915255366586</v>
+        <v>1.092661623205466</v>
       </c>
       <c r="D7" t="n">
-        <v>0.902631155346838</v>
+        <v>-0.2068012686273616</v>
       </c>
     </row>
     <row r="8">
@@ -472,13 +472,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.1447358937576115</v>
+        <v>0.06094765810494811</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.7051104763791596</v>
+        <v>-0.5887137739827044</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1649506460602129</v>
+        <v>1.113646459042408</v>
       </c>
     </row>
     <row r="9">
@@ -486,13 +486,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.08339650277274409</v>
+        <v>0.7221143501232178</v>
       </c>
       <c r="C9" t="n">
-        <v>1.075904054206959</v>
+        <v>-0.8408286765292819</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.4079888716302685</v>
+        <v>-0.5170689656819794</v>
       </c>
     </row>
     <row r="10">
@@ -500,13 +500,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.9355246062029603</v>
+        <v>-0.2268550618147382</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.694525691579211</v>
+        <v>-0.2738793612729168</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.246066658464456</v>
+        <v>0.3579536068914886</v>
       </c>
     </row>
     <row r="11">
@@ -514,13 +514,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.5428772618872022</v>
+        <v>-0.5570260025607773</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1511732992069054</v>
+        <v>0.9372762466130032</v>
       </c>
       <c r="D11" t="n">
-        <v>0.04269419488093614</v>
+        <v>0.7658316593481331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>